<commit_message>
submitted na lahat last friday
</commit_message>
<xml_diff>
--- a/Final Output/Milestone 1/Diabetes MS1/Arevalo_Nablo_Vivo_DIABETES1.xlsx
+++ b/Final Output/Milestone 1/Diabetes MS1/Arevalo_Nablo_Vivo_DIABETES1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\markarevz18\Documents (D)\Github\BSLordz\Final Output\Milestone 1\Diabetes MS1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="100" windowWidth="25620" windowHeight="13280" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="96" windowWidth="25620" windowHeight="13284" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FeatureSelectionForwardSearch" sheetId="2" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="FeatureSelectionBackwardSearch" sheetId="3" r:id="rId3"/>
     <sheet name="PCA" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="159">
   <si>
     <t>accuracy: 61.25% +/- 3.96% (mikro: 61.25%)</t>
   </si>
@@ -496,6 +501,9 @@
   </si>
   <si>
     <t>f_measure: 64.40% +/- 14.81% (mikro: 67.24%) (positive class: 1)</t>
+  </si>
+  <si>
+    <t>Top 9 PCA</t>
   </si>
 </sst>
 </file>
@@ -614,6 +622,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -908,9 +924,9 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -942,7 +958,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <v>161</v>
       </c>
@@ -953,7 +969,7 @@
         <v>0.71599999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="8" customFormat="1">
+    <row r="3" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9">
         <v>0.70189999999999997</v>
       </c>
@@ -962,7 +978,7 @@
       </c>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -994,7 +1010,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>140</v>
       </c>
@@ -1005,7 +1021,7 @@
         <v>0.75090000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="8" customFormat="1">
+    <row r="6" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9">
         <v>0.74070000000000003</v>
       </c>
@@ -1014,7 +1030,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1046,7 +1062,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>125</v>
       </c>
@@ -1057,7 +1073,7 @@
         <v>0.76890000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="8" customFormat="1">
+    <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>0.76849999999999996</v>
       </c>
@@ -1066,7 +1082,7 @@
       </c>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1098,7 +1114,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>130</v>
       </c>
@@ -1109,7 +1125,7 @@
         <v>0.75749999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="8" customFormat="1">
+    <row r="12" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9">
         <v>0.75929999999999997</v>
       </c>
@@ -1118,7 +1134,7 @@
       </c>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1150,7 +1166,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>119</v>
       </c>
@@ -1161,7 +1177,7 @@
         <v>0.76849999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="8" customFormat="1">
+    <row r="15" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="9">
         <v>0.77959999999999996</v>
       </c>
@@ -1170,7 +1186,7 @@
       </c>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1202,7 +1218,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>523</v>
       </c>
@@ -1213,7 +1229,7 @@
         <v>0.53800000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="8" customFormat="1">
+    <row r="18" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="9">
         <v>3.15E-2</v>
       </c>
@@ -1222,7 +1238,7 @@
       </c>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1254,7 +1270,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>124</v>
       </c>
@@ -1265,7 +1281,7 @@
         <v>0.73280000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="8" customFormat="1">
+    <row r="21" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="9">
         <v>0.77039999999999997</v>
       </c>
@@ -1292,9 +1308,9 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1326,7 +1342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="3">
         <v>204</v>
       </c>
@@ -1337,7 +1353,7 @@
         <v>0.64400000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="8" customFormat="1">
+    <row r="3" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6">
         <v>0.62219999999999998</v>
       </c>
@@ -1346,7 +1362,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1378,7 +1394,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>191</v>
       </c>
@@ -1389,7 +1405,7 @@
         <v>0.6583</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="8" customFormat="1">
+    <row r="6" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9">
         <v>0.64629999999999999</v>
       </c>
@@ -1398,7 +1414,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1430,7 +1446,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>183</v>
       </c>
@@ -1441,7 +1457,7 @@
         <v>0.66910000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="8" customFormat="1">
+    <row r="9" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>0.66110000000000002</v>
       </c>
@@ -1450,7 +1466,7 @@
       </c>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1482,7 +1498,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>173</v>
       </c>
@@ -1493,7 +1509,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="8" customFormat="1">
+    <row r="12" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9">
         <v>0.67959999999999998</v>
       </c>
@@ -1502,7 +1518,7 @@
       </c>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1534,7 +1550,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>176</v>
       </c>
@@ -1545,7 +1561,7 @@
         <v>0.67879999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="8" customFormat="1">
+    <row r="15" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="9">
         <v>0.67410000000000003</v>
       </c>
@@ -1554,7 +1570,7 @@
       </c>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1586,7 +1602,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>272</v>
       </c>
@@ -1597,7 +1613,7 @@
         <v>0.56269999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="8" customFormat="1">
+    <row r="18" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="9">
         <v>0.49630000000000002</v>
       </c>
@@ -1606,7 +1622,7 @@
       </c>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1638,7 +1654,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>45</v>
       </c>
@@ -1649,7 +1665,7 @@
         <v>0.81559999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="8" customFormat="1">
+    <row r="21" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="9">
         <v>0.91669999999999996</v>
       </c>
@@ -1677,65 +1693,65 @@
       <selection sqref="A1:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
     </row>
   </sheetData>
@@ -1751,22 +1767,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N1:N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>109</v>
       </c>
@@ -1785,8 +1801,14 @@
       <c r="H1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>90</v>
       </c>
@@ -1815,8 +1837,14 @@
         <f>LARGE($F$2:$H$20,J2)</f>
         <v>0.98699999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>91</v>
       </c>
@@ -1845,8 +1873,14 @@
         <f t="shared" ref="K3:K21" si="0">LARGE($F$2:$H$20,J3)</f>
         <v>0.73899999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" t="s">
+        <v>108</v>
+      </c>
+      <c r="N3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>92</v>
       </c>
@@ -1878,8 +1912,11 @@
       <c r="L4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="N4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>93</v>
       </c>
@@ -1908,8 +1945,14 @@
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" t="s">
+        <v>95</v>
+      </c>
+      <c r="N5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>94</v>
       </c>
@@ -1938,8 +1981,14 @@
         <f t="shared" si="0"/>
         <v>0.32200000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>95</v>
       </c>
@@ -1968,8 +2017,14 @@
         <f t="shared" si="0"/>
         <v>0.318</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" t="s">
+        <v>93</v>
+      </c>
+      <c r="N7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>96</v>
       </c>
@@ -1998,8 +2053,14 @@
         <f t="shared" si="0"/>
         <v>0.31</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" t="s">
+        <v>96</v>
+      </c>
+      <c r="N8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>97</v>
       </c>
@@ -2031,8 +2092,11 @@
       <c r="L9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="N9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>98</v>
       </c>
@@ -2061,8 +2125,14 @@
         <f t="shared" si="0"/>
         <v>0.29799999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" t="s">
+        <v>92</v>
+      </c>
+      <c r="N10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>99</v>
       </c>
@@ -2095,7 +2165,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>100</v>
       </c>
@@ -2128,7 +2198,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>101</v>
       </c>
@@ -2161,7 +2231,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>102</v>
       </c>
@@ -2190,8 +2260,11 @@
         <f t="shared" si="0"/>
         <v>0.247</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>103</v>
       </c>
@@ -2224,7 +2297,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>104</v>
       </c>
@@ -2257,7 +2330,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>105</v>
       </c>
@@ -2290,7 +2363,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>106</v>
       </c>
@@ -2319,8 +2392,11 @@
         <f t="shared" si="0"/>
         <v>0.121</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>107</v>
       </c>
@@ -2349,8 +2425,11 @@
         <f t="shared" si="0"/>
         <v>8.7999999999999995E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="L19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>108</v>
       </c>
@@ -2380,7 +2459,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J21">
         <v>20</v>
       </c>
@@ -2389,7 +2468,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2421,7 +2500,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B27" s="11">
         <v>187</v>
       </c>
@@ -2432,7 +2511,7 @@
         <v>0.69189999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="14">
         <v>0.65369999999999995</v>
@@ -2442,7 +2521,7 @@
       </c>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -2474,7 +2553,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30" s="11">
         <v>188</v>
       </c>
@@ -2485,7 +2564,7 @@
         <v>0.67589999999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="14">
         <v>0.65190000000000003</v>
@@ -2495,7 +2574,7 @@
       </c>
       <c r="D31" s="11"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2527,7 +2606,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B33" s="11">
         <v>173</v>
       </c>
@@ -2538,7 +2617,7 @@
         <v>0.69220000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="14">
         <v>0.67959999999999998</v>
@@ -2548,7 +2627,7 @@
       </c>
       <c r="D34" s="11"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2580,7 +2659,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B36" s="11">
         <v>161</v>
       </c>
@@ -2591,7 +2670,7 @@
         <v>0.71099999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="14">
         <v>0.70189999999999997</v>
@@ -2601,7 +2680,7 @@
       </c>
       <c r="D37" s="11"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -2633,7 +2712,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B39" s="11">
         <v>154</v>
       </c>
@@ -2644,7 +2723,7 @@
         <v>0.72150000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="14">
         <v>0.71479999999999999</v>
@@ -2654,7 +2733,7 @@
       </c>
       <c r="D40" s="11"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -2686,7 +2765,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B42" s="11">
         <v>479</v>
       </c>
@@ -2697,7 +2776,7 @@
         <v>0.53539999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="14">
         <v>0.113</v>
@@ -2707,7 +2786,7 @@
       </c>
       <c r="D43" s="11"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -2739,7 +2818,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B45" s="11">
         <v>182</v>
       </c>
@@ -2750,7 +2829,7 @@
         <v>0.64449999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
       <c r="B46" s="14">
         <v>0.66300000000000003</v>

</xml_diff>